<commit_message>
Bugfix -> Appcrash bei Änderung der Authorendaten gefixt
</commit_message>
<xml_diff>
--- a/Zeiterfassung.xlsx
+++ b/Zeiterfassung.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dditt\IdeaProjects\BIF-SS19-SWE2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87204E23-388C-4CC9-9E60-B7B5451C30F9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5CA9478-6087-4321-84A9-9679227E5E80}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Zeitliste" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="21">
   <si>
     <t>Zeiterfassung</t>
   </si>
@@ -92,6 +92,9 @@
   </si>
   <si>
     <t>Dokumentation (Javadoc) geschrieben, ConfigurationManager erstellt, Versucht das Projekt in ein JAR zu packen, aber daran gescheitert (JDBC Treiber werden nicht übernommen)</t>
+  </si>
+  <si>
+    <t>Bugfixing beim Ändern der Daten von Authoren. --&gt; Zuvor Applikations-Crash wegen endlos Schleife</t>
   </si>
 </sst>
 </file>
@@ -794,13 +797,13 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="David Dittmann" refreshedDate="43619.752623611108" refreshedVersion="6" recordCount="148" xr:uid="{00000000-000A-0000-FFFF-FFFF00000000}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="David Dittmann" refreshedDate="43620.51179409722" refreshedVersion="6" recordCount="148" xr:uid="{00000000-000A-0000-FFFF-FFFF00000000}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A5:E153" sheet="Zeitliste"/>
   </cacheSource>
   <cacheFields count="5">
     <cacheField name="Datum" numFmtId="0">
-      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2019-05-14T00:00:00" maxDate="2019-06-03T00:00:00"/>
+      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2019-05-14T00:00:00" maxDate="2019-06-04T00:00:00"/>
     </cacheField>
     <cacheField name="Ausführende/r" numFmtId="0">
       <sharedItems containsBlank="1" count="4">
@@ -824,7 +827,7 @@
       </sharedItems>
     </cacheField>
     <cacheField name="Dauer (h)" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="4" maxValue="33"/>
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="4" maxValue="38"/>
     </cacheField>
     <cacheField name="Anmerkung" numFmtId="0">
       <sharedItems containsBlank="1"/>
@@ -876,11 +879,11 @@
     <s v="Bildergallerie added, AuthorenManager added, Validierung von Authoren / Bilderdaten im BL added, Suchfunktion nach Keywords added --&gt; PROBLEM: PUSH NICHT MÖGLICH!"/>
   </r>
   <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
+    <d v="2019-06-03T00:00:00"/>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="5"/>
+    <s v="Dokumentation (Javadoc) geschrieben, ConfigurationManager erstellt, Versucht das Projekt in ein JAR zu packen, aber daran gescheitert (JDBC Treiber werden nicht übernommen)"/>
   </r>
   <r>
     <m/>
@@ -942,7 +945,7 @@
     <m/>
     <x v="1"/>
     <x v="3"/>
-    <n v="33"/>
+    <n v="38"/>
     <m/>
   </r>
   <r>
@@ -2241,7 +2244,7 @@
   <dimension ref="A1:E157"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2402,11 +2405,21 @@
       </c>
     </row>
     <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="5"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="6"/>
+      <c r="A12" s="14">
+        <v>43620</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="5">
+        <v>1</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="7"/>
@@ -2465,7 +2478,7 @@
       </c>
       <c r="D20" s="7">
         <f>SUM(D6:D17)</f>
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E20" s="8"/>
     </row>

</xml_diff>

<commit_message>
Letzte testings (keine unittests), ersatzbereicht geschrieben
</commit_message>
<xml_diff>
--- a/Zeiterfassung.xlsx
+++ b/Zeiterfassung.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dditt\IdeaProjects\BIF-SS19-SWE2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dditt\IdeaProjects\BIF-SS19-SWE2-origin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5CA9478-6087-4321-84A9-9679227E5E80}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{295DE2A8-9638-4C4F-8157-F1B291B1DA21}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Zeitliste" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="23">
   <si>
     <t>Zeiterfassung</t>
   </si>
@@ -85,16 +85,22 @@
     <t>Summe:</t>
   </si>
   <si>
-    <t>Überarbeitung DAL, Presentationmodels erstellt, Datamodels angepasst, binding der presentationmodels zum GUI, Anzeige des ersten Bildes und der dazugehörigen Daten</t>
-  </si>
-  <si>
     <t>Bildergallerie added, AuthorenManager added, Validierung von Authoren / Bilderdaten im BL added, Suchfunktion nach Keywords added --&gt; PROBLEM: PUSH NICHT MÖGLICH!</t>
   </si>
   <si>
-    <t>Dokumentation (Javadoc) geschrieben, ConfigurationManager erstellt, Versucht das Projekt in ein JAR zu packen, aber daran gescheitert (JDBC Treiber werden nicht übernommen)</t>
+    <t>Bugfixing beim Ändern der Daten von Authoren. --&gt; Zuvor Applikations-Crash wegen endlos Schleife</t>
   </si>
   <si>
-    <t>Bugfixing beim Ändern der Daten von Authoren. --&gt; Zuvor Applikations-Crash wegen endlos Schleife</t>
+    <t>Management</t>
+  </si>
+  <si>
+    <t>Ersatzbericht geschrieben, Dokumentation angepasst, Abschluss Bericht geschrieben</t>
+  </si>
+  <si>
+    <t>Dokumentation (Javadoc) geschrieben, ConfigurationManager erstellt, Versucht das Projekt in ein JAR zu packen, aber daran gescheitert (JDBC Treiber wird nicht übernommen)</t>
+  </si>
+  <si>
+    <t>komplette Überarbeitung DAL, Presentationmodels erstellt, Datamodels angepasst, binding der presentationmodels zum GUI, Anzeige des ersten Bildes und der dazugehörigen Daten</t>
   </si>
 </sst>
 </file>
@@ -797,13 +803,13 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="David Dittmann" refreshedDate="43620.51179409722" refreshedVersion="6" recordCount="148" xr:uid="{00000000-000A-0000-FFFF-FFFF00000000}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="David Dittmann" refreshedDate="43620.707195370371" refreshedVersion="6" recordCount="148" xr:uid="{00000000-000A-0000-FFFF-FFFF00000000}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A5:E153" sheet="Zeitliste"/>
   </cacheSource>
   <cacheFields count="5">
     <cacheField name="Datum" numFmtId="0">
-      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2019-05-14T00:00:00" maxDate="2019-06-04T00:00:00"/>
+      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2019-05-14T00:00:00" maxDate="2019-06-05T00:00:00"/>
     </cacheField>
     <cacheField name="Ausführende/r" numFmtId="0">
       <sharedItems containsBlank="1" count="4">
@@ -827,7 +833,7 @@
       </sharedItems>
     </cacheField>
     <cacheField name="Dauer (h)" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="4" maxValue="38"/>
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="1" maxValue="39"/>
     </cacheField>
     <cacheField name="Anmerkung" numFmtId="0">
       <sharedItems containsBlank="1"/>
@@ -886,11 +892,11 @@
     <s v="Dokumentation (Javadoc) geschrieben, ConfigurationManager erstellt, Versucht das Projekt in ein JAR zu packen, aber daran gescheitert (JDBC Treiber werden nicht übernommen)"/>
   </r>
   <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
+    <d v="2019-06-04T00:00:00"/>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="1"/>
+    <s v="Bugfixing beim Ändern der Daten von Authoren. --&gt; Zuvor Applikations-Crash wegen endlos Schleife"/>
   </r>
   <r>
     <m/>
@@ -945,7 +951,7 @@
     <m/>
     <x v="1"/>
     <x v="3"/>
-    <n v="38"/>
+    <n v="39"/>
     <m/>
   </r>
   <r>
@@ -2244,7 +2250,7 @@
   <dimension ref="A1:E157"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2367,7 +2373,7 @@
         <v>10</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
@@ -2381,10 +2387,10 @@
         <v>7</v>
       </c>
       <c r="D10" s="5">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
@@ -2401,7 +2407,7 @@
         <v>5</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2418,15 +2424,25 @@
         <v>1</v>
       </c>
       <c r="E12" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="14">
+        <v>43620</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="7">
+        <v>3</v>
+      </c>
+      <c r="E13" s="8" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="7"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="8"/>
     </row>
     <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="7"/>
@@ -2478,7 +2494,7 @@
       </c>
       <c r="D20" s="7">
         <f>SUM(D6:D17)</f>
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="E20" s="8"/>
     </row>

</xml_diff>

<commit_message>
Logging added, rudimentaeres testen des loggings
</commit_message>
<xml_diff>
--- a/Zeiterfassung.xlsx
+++ b/Zeiterfassung.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dditt\IdeaProjects\BIF-SS19-SWE2-origin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{295DE2A8-9638-4C4F-8157-F1B291B1DA21}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC2FB7E3-FC97-470A-B0FA-D2E4852510A6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -91,16 +91,16 @@
     <t>Bugfixing beim Ändern der Daten von Authoren. --&gt; Zuvor Applikations-Crash wegen endlos Schleife</t>
   </si>
   <si>
-    <t>Management</t>
-  </si>
-  <si>
-    <t>Ersatzbericht geschrieben, Dokumentation angepasst, Abschluss Bericht geschrieben</t>
-  </si>
-  <si>
     <t>Dokumentation (Javadoc) geschrieben, ConfigurationManager erstellt, Versucht das Projekt in ein JAR zu packen, aber daran gescheitert (JDBC Treiber wird nicht übernommen)</t>
   </si>
   <si>
     <t>komplette Überarbeitung DAL, Presentationmodels erstellt, Datamodels angepasst, binding der presentationmodels zum GUI, Anzeige des ersten Bildes und der dazugehörigen Daten</t>
+  </si>
+  <si>
+    <t>Logging, Ersatzbericht geschrieben, Dokumentation angepasst, Abschluss Bericht geschrieben</t>
+  </si>
+  <si>
+    <t>Developement / Management</t>
   </si>
 </sst>
 </file>
@@ -803,7 +803,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="David Dittmann" refreshedDate="43620.707195370371" refreshedVersion="6" recordCount="148" xr:uid="{00000000-000A-0000-FFFF-FFFF00000000}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="David Dittmann" refreshedDate="43620.860499537041" refreshedVersion="6" recordCount="148" xr:uid="{00000000-000A-0000-FFFF-FFFF00000000}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A5:E153" sheet="Zeitliste"/>
   </cacheSource>
@@ -820,9 +820,10 @@
       </sharedItems>
     </cacheField>
     <cacheField name="Tätigkeit" numFmtId="0">
-      <sharedItems containsBlank="1" count="9">
+      <sharedItems containsBlank="1" count="10">
         <s v="Projekteinrichtung"/>
         <s v="Development"/>
+        <s v="Developement / Management"/>
         <m/>
         <s v="Summe:"/>
         <s v="Deployment" u="1"/>
@@ -833,7 +834,7 @@
       </sharedItems>
     </cacheField>
     <cacheField name="Dauer (h)" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="1" maxValue="39"/>
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="1" maxValue="45"/>
     </cacheField>
     <cacheField name="Anmerkung" numFmtId="0">
       <sharedItems containsBlank="1"/>
@@ -875,13 +876,13 @@
     <x v="0"/>
     <x v="1"/>
     <n v="10"/>
-    <s v="Überarbeitung DAL, Presentationmodels erstellt, Datamodels angepasst, binding der presentationmodels zum GUI, Anzeige des ersten Bildes und der dazugehörigen Daten"/>
+    <s v="komplette Überarbeitung DAL, Presentationmodels erstellt, Datamodels angepasst, binding der presentationmodels zum GUI, Anzeige des ersten Bildes und der dazugehörigen Daten"/>
   </r>
   <r>
     <d v="2019-06-02T00:00:00"/>
     <x v="0"/>
     <x v="1"/>
-    <n v="7"/>
+    <n v="8"/>
     <s v="Bildergallerie added, AuthorenManager added, Validierung von Authoren / Bilderdaten im BL added, Suchfunktion nach Keywords added --&gt; PROBLEM: PUSH NICHT MÖGLICH!"/>
   </r>
   <r>
@@ -889,7 +890,7 @@
     <x v="0"/>
     <x v="1"/>
     <n v="5"/>
-    <s v="Dokumentation (Javadoc) geschrieben, ConfigurationManager erstellt, Versucht das Projekt in ein JAR zu packen, aber daran gescheitert (JDBC Treiber werden nicht übernommen)"/>
+    <s v="Dokumentation (Javadoc) geschrieben, ConfigurationManager erstellt, Versucht das Projekt in ein JAR zu packen, aber daran gescheitert (JDBC Treiber wird nicht übernommen)"/>
   </r>
   <r>
     <d v="2019-06-04T00:00:00"/>
@@ -899,989 +900,989 @@
     <s v="Bugfixing beim Ändern der Daten von Authoren. --&gt; Zuvor Applikations-Crash wegen endlos Schleife"/>
   </r>
   <r>
-    <m/>
-    <x v="1"/>
+    <d v="2019-06-04T00:00:00"/>
+    <x v="0"/>
     <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="3"/>
-    <n v="39"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <x v="2"/>
+    <n v="5"/>
+    <s v="Logging, Ersatzbericht geschrieben, Dokumentation angepasst, Abschluss Bericht geschrieben"/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="4"/>
+    <n v="45"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="1"/>
+    <x v="3"/>
     <m/>
     <m/>
   </r>
@@ -1903,16 +1904,17 @@
       </items>
     </pivotField>
     <pivotField name="Tätigkeit" axis="axisRow" compact="0" outline="0" multipleItemSelectionAllowed="1" showAll="0" sortType="ascending">
-      <items count="10">
-        <item m="1" x="4"/>
+      <items count="11">
+        <item m="1" x="5"/>
+        <item x="2"/>
         <item x="1"/>
+        <item m="1" x="9"/>
+        <item m="1" x="6"/>
+        <item x="0"/>
         <item m="1" x="8"/>
-        <item m="1" x="5"/>
-        <item x="0"/>
+        <item x="4"/>
         <item m="1" x="7"/>
         <item x="3"/>
-        <item m="1" x="6"/>
-        <item x="2"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -2250,7 +2252,7 @@
   <dimension ref="A1:E157"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2373,7 +2375,7 @@
         <v>10</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
@@ -2407,7 +2409,7 @@
         <v>5</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2427,7 +2429,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A13" s="14">
         <v>43620</v>
       </c>
@@ -2435,13 +2437,13 @@
         <v>11</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D13" s="7">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2494,7 +2496,7 @@
       </c>
       <c r="D20" s="7">
         <f>SUM(D6:D17)</f>
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E20" s="8"/>
     </row>

</xml_diff>